<commit_message>
separating into individual service, app and lib
</commit_message>
<xml_diff>
--- a/excelDocs/scarletAndViolet151/pokemon_data.xlsx
+++ b/excelDocs/scarletAndViolet151/pokemon_data.xlsx
@@ -664,7 +664,7 @@
         <v>46</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>0.16</v>
@@ -682,20 +682,20 @@
         <v/>
       </c>
       <c r="I2" s="3" t="n">
-        <v>9.890000000000001</v>
+        <v>9.99</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>65.48999999999999</v>
+        <v>65.69</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>232.98</v>
+        <v>233.43</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>6.19</v>
+        <v>6.35</v>
       </c>
       <c r="M2" s="3" t="n"/>
       <c r="N2" s="3" t="n">
-        <v>372.92</v>
+        <v>373.94</v>
       </c>
       <c r="R2" s="3" t="n"/>
       <c r="S2" s="3" t="n"/>
@@ -733,7 +733,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>0.59</v>
@@ -789,7 +789,7 @@
         <v>90</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.92</v>
+        <v>0.98</v>
       </c>
       <c r="E4" s="3" t="inlineStr"/>
       <c r="F4" s="3">
@@ -843,7 +843,7 @@
         <v>248</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>7.01</v>
+        <v>6.63</v>
       </c>
       <c r="E5" s="3" t="inlineStr"/>
       <c r="F5" s="3">
@@ -897,7 +897,7 @@
         <v>225</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>36.5</v>
+        <v>36.92</v>
       </c>
       <c r="E6" s="3" t="inlineStr"/>
       <c r="F6" s="3">
@@ -954,7 +954,7 @@
         <v>0.1</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.48</v>
       </c>
       <c r="F7" s="3">
         <f>IF(B7:B215="common", 4, IF(B7:B215="uncommon", 3, IF(B7:B215="rare", 0.792892156862745, 1)))</f>
@@ -1010,7 +1010,7 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.95</v>
+        <v>1.02</v>
       </c>
       <c r="F8" s="3">
         <f>IF(B8:B216="common", 4, IF(B8:B216="uncommon", 3, IF(B8:B216="rare", 0.792892156862745, 1)))</f>
@@ -1066,7 +1066,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.61</v>
+        <v>0.58</v>
       </c>
       <c r="F9" s="3">
         <f>IF(B9:B217="common", 4, IF(B9:B217="uncommon", 3, IF(B9:B217="rare", 0.792892156862745, 1)))</f>
@@ -1173,7 +1173,7 @@
         <v>248</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>4.77</v>
+        <v>4.3</v>
       </c>
       <c r="E11" s="3" t="inlineStr"/>
       <c r="F11" s="3">
@@ -1224,7 +1224,7 @@
         <v>33</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>0.14</v>
@@ -1277,10 +1277,10 @@
         <v>21</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
       <c r="F13" s="3">
         <f>IF(B13:B221="common", 4, IF(B13:B221="uncommon", 3, IF(B13:B221="rare", 0.792892156862745, 1)))</f>
@@ -1330,7 +1330,7 @@
         <v>154</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>4.45</v>
+        <v>4.07</v>
       </c>
       <c r="E14" s="3" t="inlineStr"/>
       <c r="F14" s="3">
@@ -1384,7 +1384,7 @@
         <v>0.14</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="F15" s="3">
         <f>IF(B15:B223="common", 4, IF(B15:B223="uncommon", 3, IF(B15:B223="rare", 0.792892156862745, 1)))</f>
@@ -1487,10 +1487,10 @@
         <v>33</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="F17" s="3">
         <f>IF(B17:B225="common", 4, IF(B17:B225="uncommon", 3, IF(B17:B225="rare", 0.792892156862745, 1)))</f>
@@ -1540,10 +1540,10 @@
         <v>33</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>0.39</v>
+        <v>0.42</v>
       </c>
       <c r="F18" s="3">
         <f>IF(B18:B226="common", 4, IF(B18:B226="uncommon", 3, IF(B18:B226="rare", 0.792892156862745, 1)))</f>
@@ -1593,7 +1593,7 @@
         <v>248</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>2.85</v>
+        <v>2.76</v>
       </c>
       <c r="E19" s="3" t="inlineStr"/>
       <c r="F19" s="3">
@@ -1644,7 +1644,7 @@
         <v>90</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>0.85</v>
+        <v>0.72</v>
       </c>
       <c r="E20" s="3" t="inlineStr"/>
       <c r="F20" s="3">
@@ -1746,7 +1746,7 @@
         <v>225</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>65.44</v>
+        <v>65.77</v>
       </c>
       <c r="E22" s="3" t="inlineStr"/>
       <c r="F22" s="3">
@@ -1797,7 +1797,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>0.16</v>
@@ -1850,7 +1850,7 @@
         <v>188</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>34.08</v>
+        <v>34.47</v>
       </c>
       <c r="E24" s="3" t="inlineStr"/>
       <c r="F24" s="3">
@@ -1904,7 +1904,7 @@
         <v>0.06</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="F25" s="3">
         <f>IF(B25:B233="common", 4, IF(B25:B233="uncommon", 3, IF(B25:B233="rare", 0.792892156862745, 1)))</f>
@@ -1954,7 +1954,7 @@
         <v>46</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>0.19</v>
@@ -2007,7 +2007,7 @@
         <v>188</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>7.19</v>
+        <v>6.72</v>
       </c>
       <c r="E27" s="3" t="inlineStr"/>
       <c r="F27" s="3">
@@ -2058,10 +2058,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="F28" s="3">
         <f>IF(B28:B236="common", 4, IF(B28:B236="uncommon", 3, IF(B28:B236="rare", 0.792892156862745, 1)))</f>
@@ -2111,7 +2111,7 @@
         <v>90</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>4.25</v>
+        <v>4.47</v>
       </c>
       <c r="E29" s="3" t="inlineStr"/>
       <c r="F29" s="3">
@@ -2162,7 +2162,7 @@
         <v>248</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>26.9</v>
+        <v>27.01</v>
       </c>
       <c r="E30" s="3" t="inlineStr"/>
       <c r="F30" s="3">
@@ -2213,7 +2213,7 @@
         <v>225</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>198.4</v>
+        <v>198.68</v>
       </c>
       <c r="E31" s="3" t="inlineStr"/>
       <c r="F31" s="3">
@@ -2264,10 +2264,10 @@
         <v>46</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E32" s="3" t="n">
-        <v>0.24</v>
+        <v>0.45</v>
       </c>
       <c r="F32" s="3">
         <f>IF(B32:B240="common", 4, IF(B32:B240="uncommon", 3, IF(B32:B240="rare", 0.792892156862745, 1)))</f>
@@ -2368,10 +2368,10 @@
         <v>33</v>
       </c>
       <c r="D34" s="3" t="n">
-        <v>0.08</v>
+        <v>0.27</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F34" s="3">
         <f>IF(B34:B242="common", 4, IF(B34:B242="uncommon", 3, IF(B34:B242="rare", 0.792892156862745, 1)))</f>
@@ -2421,7 +2421,7 @@
         <v>188</v>
       </c>
       <c r="D35" s="3" t="n">
-        <v>32.18</v>
+        <v>32.91</v>
       </c>
       <c r="E35" s="3" t="inlineStr"/>
       <c r="F35" s="3">
@@ -2472,7 +2472,7 @@
         <v>33</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E36" s="3" t="n">
         <v>0.23</v>
@@ -2528,7 +2528,7 @@
         <v>0.06</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="F37" s="3">
         <f>IF(B37:B245="common", 4, IF(B37:B245="uncommon", 3, IF(B37:B245="rare", 0.792892156862745, 1)))</f>
@@ -2578,7 +2578,7 @@
         <v>33</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>0.18</v>
@@ -2634,7 +2634,7 @@
         <v>0.06</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="F39" s="3">
         <f>IF(B39:B247="common", 4, IF(B39:B247="uncommon", 3, IF(B39:B247="rare", 0.792892156862745, 1)))</f>
@@ -2684,10 +2684,10 @@
         <v>33</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E40" s="3" t="n">
-        <v>0.66</v>
+        <v>0.71</v>
       </c>
       <c r="F40" s="3">
         <f>IF(B40:B248="common", 4, IF(B40:B248="uncommon", 3, IF(B40:B248="rare", 0.792892156862745, 1)))</f>
@@ -2737,10 +2737,10 @@
         <v>33</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>0.64</v>
+        <v>0.66</v>
       </c>
       <c r="F41" s="3">
         <f>IF(B41:B249="common", 4, IF(B41:B249="uncommon", 3, IF(B41:B249="rare", 0.792892156862745, 1)))</f>
@@ -2790,7 +2790,7 @@
         <v>248</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>3.26</v>
+        <v>3.27</v>
       </c>
       <c r="E42" s="3" t="inlineStr"/>
       <c r="F42" s="3">
@@ -2947,7 +2947,7 @@
         <v>21</v>
       </c>
       <c r="D45" s="3" t="n">
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
       <c r="E45" s="3" t="n">
         <v>0.65</v>
@@ -3000,7 +3000,7 @@
         <v>21</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
       <c r="E46" s="3" t="inlineStr"/>
       <c r="F46" s="3">
@@ -3051,10 +3051,10 @@
         <v>21</v>
       </c>
       <c r="D47" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="F47" s="3">
         <f>IF(B47:B255="common", 4, IF(B47:B255="uncommon", 3, IF(B47:B255="rare", 0.792892156862745, 1)))</f>
@@ -3107,7 +3107,7 @@
         <v>0.06</v>
       </c>
       <c r="E48" s="3" t="n">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="F48" s="3">
         <f>IF(B48:B256="common", 4, IF(B48:B256="uncommon", 3, IF(B48:B256="rare", 0.792892156862745, 1)))</f>
@@ -3160,7 +3160,7 @@
         <v>0.11</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>1.67</v>
+        <v>1.69</v>
       </c>
       <c r="F49" s="3">
         <f>IF(B49:B257="common", 4, IF(B49:B257="uncommon", 3, IF(B49:B257="rare", 0.792892156862745, 1)))</f>
@@ -3210,7 +3210,7 @@
         <v>188</v>
       </c>
       <c r="D50" s="3" t="n">
-        <v>20.51</v>
+        <v>20.52</v>
       </c>
       <c r="E50" s="3" t="inlineStr"/>
       <c r="F50" s="3">
@@ -3261,7 +3261,7 @@
         <v>21</v>
       </c>
       <c r="D51" s="3" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="E51" s="3" t="n">
         <v>1.37</v>
@@ -3314,10 +3314,10 @@
         <v>46</v>
       </c>
       <c r="D52" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="F52" s="3">
         <f>IF(B52:B260="common", 4, IF(B52:B260="uncommon", 3, IF(B52:B260="rare", 0.792892156862745, 1)))</f>
@@ -3423,7 +3423,7 @@
         <v>0.05</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F54" s="3">
         <f>IF(B54:B262="common", 4, IF(B54:B262="uncommon", 3, IF(B54:B262="rare", 0.792892156862745, 1)))</f>
@@ -3473,10 +3473,10 @@
         <v>46</v>
       </c>
       <c r="D55" s="3" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="F55" s="3">
         <f>IF(B55:B263="common", 4, IF(B55:B263="uncommon", 3, IF(B55:B263="rare", 0.792892156862745, 1)))</f>
@@ -3526,7 +3526,7 @@
         <v>46</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E56" s="3" t="n">
         <v>0.16</v>
@@ -3579,10 +3579,10 @@
         <v>46</v>
       </c>
       <c r="D57" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E57" s="3" t="n">
-        <v>0.58</v>
+        <v>0.51</v>
       </c>
       <c r="F57" s="3">
         <f>IF(B57:B265="common", 4, IF(B57:B265="uncommon", 3, IF(B57:B265="rare", 0.792892156862745, 1)))</f>
@@ -3632,10 +3632,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="3" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="E58" s="3" t="n">
-        <v>1.14</v>
+        <v>1.11</v>
       </c>
       <c r="F58" s="3">
         <f>IF(B58:B266="common", 4, IF(B58:B266="uncommon", 3, IF(B58:B266="rare", 0.792892156862745, 1)))</f>
@@ -3688,7 +3688,7 @@
         <v>0.14</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>1.11</v>
+        <v>1.12</v>
       </c>
       <c r="F59" s="3">
         <f>IF(B59:B267="common", 4, IF(B59:B267="uncommon", 3, IF(B59:B267="rare", 0.792892156862745, 1)))</f>
@@ -3741,7 +3741,7 @@
         <v>0.09</v>
       </c>
       <c r="E60" s="3" t="n">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="F60" s="3">
         <f>IF(B60:B268="common", 4, IF(B60:B268="uncommon", 3, IF(B60:B268="rare", 0.792892156862745, 1)))</f>
@@ -3791,7 +3791,7 @@
         <v>248</v>
       </c>
       <c r="D61" s="3" t="n">
-        <v>5.73</v>
+        <v>5.75</v>
       </c>
       <c r="E61" s="3" t="inlineStr"/>
       <c r="F61" s="3">
@@ -3842,7 +3842,7 @@
         <v>225</v>
       </c>
       <c r="D62" s="3" t="n">
-        <v>13.57</v>
+        <v>13.1</v>
       </c>
       <c r="E62" s="3" t="inlineStr"/>
       <c r="F62" s="3">
@@ -3893,10 +3893,10 @@
         <v>46</v>
       </c>
       <c r="D63" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F63" s="3">
         <f>IF(B63:B271="common", 4, IF(B63:B271="uncommon", 3, IF(B63:B271="rare", 0.792892156862745, 1)))</f>
@@ -3949,7 +3949,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E64" s="3" t="n">
-        <v>1.5</v>
+        <v>1.51</v>
       </c>
       <c r="F64" s="3">
         <f>IF(B64:B272="common", 4, IF(B64:B272="uncommon", 3, IF(B64:B272="rare", 0.792892156862745, 1)))</f>
@@ -4055,7 +4055,7 @@
         <v>0.06</v>
       </c>
       <c r="E66" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F66" s="3">
         <f>IF(B66:B274="common", 4, IF(B66:B274="uncommon", 3, IF(B66:B274="rare", 0.792892156862745, 1)))</f>
@@ -4105,10 +4105,10 @@
         <v>21</v>
       </c>
       <c r="D67" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>1.07</v>
+        <v>0.98</v>
       </c>
       <c r="F67" s="3">
         <f>IF(B67:B275="common", 4, IF(B67:B275="uncommon", 3, IF(B67:B275="rare", 0.792892156862745, 1)))</f>
@@ -4158,10 +4158,10 @@
         <v>46</v>
       </c>
       <c r="D68" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E68" s="3" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="F68" s="3">
         <f>IF(B68:B276="common", 4, IF(B68:B276="uncommon", 3, IF(B68:B276="rare", 0.792892156862745, 1)))</f>
@@ -4211,10 +4211,10 @@
         <v>21</v>
       </c>
       <c r="D69" s="3" t="n">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>2.02</v>
+        <v>1.96</v>
       </c>
       <c r="F69" s="3">
         <f>IF(B69:B277="common", 4, IF(B69:B277="uncommon", 3, IF(B69:B277="rare", 0.792892156862745, 1)))</f>
@@ -4267,7 +4267,7 @@
         <v>0.04</v>
       </c>
       <c r="E70" s="3" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="F70" s="3">
         <f>IF(B70:B278="common", 4, IF(B70:B278="uncommon", 3, IF(B70:B278="rare", 0.792892156862745, 1)))</f>
@@ -4317,10 +4317,10 @@
         <v>33</v>
       </c>
       <c r="D71" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E71" s="3" t="n">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="F71" s="3">
         <f>IF(B71:B279="common", 4, IF(B71:B279="uncommon", 3, IF(B71:B279="rare", 0.792892156862745, 1)))</f>
@@ -4370,7 +4370,7 @@
         <v>248</v>
       </c>
       <c r="D72" s="3" t="n">
-        <v>4.94</v>
+        <v>4.48</v>
       </c>
       <c r="E72" s="3" t="inlineStr"/>
       <c r="F72" s="3">
@@ -4421,7 +4421,7 @@
         <v>225</v>
       </c>
       <c r="D73" s="3" t="n">
-        <v>12.87</v>
+        <v>13.06</v>
       </c>
       <c r="E73" s="3" t="inlineStr"/>
       <c r="F73" s="3">
@@ -4472,10 +4472,10 @@
         <v>33</v>
       </c>
       <c r="D74" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F74" s="3">
         <f>IF(B74:B282="common", 4, IF(B74:B282="uncommon", 3, IF(B74:B282="rare", 0.792892156862745, 1)))</f>
@@ -4525,7 +4525,7 @@
         <v>33</v>
       </c>
       <c r="D75" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E75" s="3" t="n">
         <v>0.18</v>
@@ -4578,10 +4578,10 @@
         <v>46</v>
       </c>
       <c r="D76" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E76" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F76" s="3">
         <f>IF(B76:B284="common", 4, IF(B76:B284="uncommon", 3, IF(B76:B284="rare", 0.792892156862745, 1)))</f>
@@ -4684,7 +4684,7 @@
         <v>90</v>
       </c>
       <c r="D78" s="3" t="n">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="E78" s="3" t="inlineStr"/>
       <c r="F78" s="3">
@@ -4735,7 +4735,7 @@
         <v>248</v>
       </c>
       <c r="D79" s="3" t="n">
-        <v>5.26</v>
+        <v>4.9</v>
       </c>
       <c r="E79" s="3" t="inlineStr"/>
       <c r="F79" s="3">
@@ -4789,7 +4789,7 @@
         <v>0.12</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>0.6</v>
+        <v>0.58</v>
       </c>
       <c r="F80" s="3">
         <f>IF(B80:B288="common", 4, IF(B80:B288="uncommon", 3, IF(B80:B288="rare", 0.792892156862745, 1)))</f>
@@ -4945,10 +4945,10 @@
         <v>46</v>
       </c>
       <c r="D83" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E83" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F83" s="3">
         <f>IF(B83:B291="common", 4, IF(B83:B291="uncommon", 3, IF(B83:B291="rare", 0.792892156862745, 1)))</f>
@@ -4998,7 +4998,7 @@
         <v>21</v>
       </c>
       <c r="D84" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="E84" s="3" t="n">
         <v>0.93</v>
@@ -5104,10 +5104,10 @@
         <v>33</v>
       </c>
       <c r="D86" s="3" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>1.2</v>
+        <v>1.22</v>
       </c>
       <c r="F86" s="3">
         <f>IF(B86:B294="common", 4, IF(B86:B294="uncommon", 3, IF(B86:B294="rare", 0.792892156862745, 1)))</f>
@@ -5157,10 +5157,10 @@
         <v>33</v>
       </c>
       <c r="D87" s="3" t="n">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="E87" s="3" t="n">
-        <v>1.25</v>
+        <v>1.27</v>
       </c>
       <c r="F87" s="3">
         <f>IF(B87:B295="common", 4, IF(B87:B295="uncommon", 3, IF(B87:B295="rare", 0.792892156862745, 1)))</f>
@@ -5210,10 +5210,10 @@
         <v>46</v>
       </c>
       <c r="D88" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E88" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F88" s="3">
         <f>IF(B88:B296="common", 4, IF(B88:B296="uncommon", 3, IF(B88:B296="rare", 0.792892156862745, 1)))</f>
@@ -5263,10 +5263,10 @@
         <v>33</v>
       </c>
       <c r="D89" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E89" s="3" t="n">
-        <v>1.05</v>
+        <v>0.98</v>
       </c>
       <c r="F89" s="3">
         <f>IF(B89:B297="common", 4, IF(B89:B297="uncommon", 3, IF(B89:B297="rare", 0.792892156862745, 1)))</f>
@@ -5319,7 +5319,7 @@
         <v>0.1</v>
       </c>
       <c r="E90" s="3" t="n">
-        <v>0.28</v>
+        <v>0.26</v>
       </c>
       <c r="F90" s="3">
         <f>IF(B90:B298="common", 4, IF(B90:B298="uncommon", 3, IF(B90:B298="rare", 0.792892156862745, 1)))</f>
@@ -5369,7 +5369,7 @@
         <v>188</v>
       </c>
       <c r="D91" s="3" t="n">
-        <v>27.76</v>
+        <v>27.56</v>
       </c>
       <c r="E91" s="3" t="inlineStr"/>
       <c r="F91" s="3">
@@ -5423,7 +5423,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E92" s="3" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="F92" s="3">
         <f>IF(B92:B300="common", 4, IF(B92:B300="uncommon", 3, IF(B92:B300="rare", 0.792892156862745, 1)))</f>
@@ -5473,10 +5473,10 @@
         <v>21</v>
       </c>
       <c r="D93" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="E93" s="3" t="n">
-        <v>2.14</v>
+        <v>2.03</v>
       </c>
       <c r="F93" s="3">
         <f>IF(B93:B301="common", 4, IF(B93:B301="uncommon", 3, IF(B93:B301="rare", 0.792892156862745, 1)))</f>
@@ -5526,7 +5526,7 @@
         <v>90</v>
       </c>
       <c r="D94" s="3" t="n">
-        <v>0.82</v>
+        <v>0.96</v>
       </c>
       <c r="E94" s="3" t="inlineStr"/>
       <c r="F94" s="3">
@@ -5577,7 +5577,7 @@
         <v>248</v>
       </c>
       <c r="D95" s="3" t="n">
-        <v>4.23</v>
+        <v>4.2</v>
       </c>
       <c r="E95" s="3" t="inlineStr"/>
       <c r="F95" s="3">
@@ -5628,10 +5628,10 @@
         <v>33</v>
       </c>
       <c r="D96" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E96" s="3" t="n">
-        <v>1.1</v>
+        <v>1.13</v>
       </c>
       <c r="F96" s="3">
         <f>IF(B96:B304="common", 4, IF(B96:B304="uncommon", 3, IF(B96:B304="rare", 0.792892156862745, 1)))</f>
@@ -5684,7 +5684,7 @@
         <v>0.14</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>0.96</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F97" s="3">
         <f>IF(B97:B305="common", 4, IF(B97:B305="uncommon", 3, IF(B97:B305="rare", 0.792892156862745, 1)))</f>
@@ -5737,7 +5737,7 @@
         <v>0.05</v>
       </c>
       <c r="E98" s="3" t="n">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="F98" s="3">
         <f>IF(B98:B306="common", 4, IF(B98:B306="uncommon", 3, IF(B98:B306="rare", 0.792892156862745, 1)))</f>
@@ -5840,7 +5840,7 @@
         <v>90</v>
       </c>
       <c r="D100" s="3" t="n">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="E100" s="3" t="inlineStr"/>
       <c r="F100" s="3">
@@ -5891,7 +5891,7 @@
         <v>248</v>
       </c>
       <c r="D101" s="3" t="n">
-        <v>4.89</v>
+        <v>4.75</v>
       </c>
       <c r="E101" s="3" t="inlineStr"/>
       <c r="F101" s="3">
@@ -5945,7 +5945,7 @@
         <v>0.06</v>
       </c>
       <c r="E102" s="3" t="n">
-        <v>1.41</v>
+        <v>1.43</v>
       </c>
       <c r="F102" s="3">
         <f>IF(B102:B310="common", 4, IF(B102:B310="uncommon", 3, IF(B102:B310="rare", 0.792892156862745, 1)))</f>
@@ -5995,7 +5995,7 @@
         <v>46</v>
       </c>
       <c r="D103" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E103" s="3" t="n">
         <v>0.13</v>
@@ -6048,10 +6048,10 @@
         <v>46</v>
       </c>
       <c r="D104" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E104" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F104" s="3">
         <f>IF(B104:B312="common", 4, IF(B104:B312="uncommon", 3, IF(B104:B312="rare", 0.792892156862745, 1)))</f>
@@ -6104,7 +6104,7 @@
         <v>0.09</v>
       </c>
       <c r="E105" s="3" t="n">
-        <v>1.27</v>
+        <v>1.18</v>
       </c>
       <c r="F105" s="3">
         <f>IF(B105:B313="common", 4, IF(B105:B313="uncommon", 3, IF(B105:B313="rare", 0.792892156862745, 1)))</f>
@@ -6154,7 +6154,7 @@
         <v>33</v>
       </c>
       <c r="D106" s="3" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="E106" s="3" t="n">
         <v>0.51</v>
@@ -6260,10 +6260,10 @@
         <v>21</v>
       </c>
       <c r="D108" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="E108" s="3" t="n">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="F108" s="3">
         <f>IF(B108:B316="common", 4, IF(B108:B316="uncommon", 3, IF(B108:B316="rare", 0.792892156862745, 1)))</f>
@@ -6313,10 +6313,10 @@
         <v>33</v>
       </c>
       <c r="D109" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E109" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="F109" s="3">
         <f>IF(B109:B317="common", 4, IF(B109:B317="uncommon", 3, IF(B109:B317="rare", 0.792892156862745, 1)))</f>
@@ -6366,7 +6366,7 @@
         <v>188</v>
       </c>
       <c r="D110" s="3" t="n">
-        <v>9.869999999999999</v>
+        <v>10.21</v>
       </c>
       <c r="E110" s="3" t="inlineStr"/>
       <c r="F110" s="3">
@@ -6417,10 +6417,10 @@
         <v>46</v>
       </c>
       <c r="D111" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E111" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F111" s="3">
         <f>IF(B111:B319="common", 4, IF(B111:B319="uncommon", 3, IF(B111:B319="rare", 0.792892156862745, 1)))</f>
@@ -6523,10 +6523,10 @@
         <v>46</v>
       </c>
       <c r="D113" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E113" s="3" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.93</v>
       </c>
       <c r="F113" s="3">
         <f>IF(B113:B321="common", 4, IF(B113:B321="uncommon", 3, IF(B113:B321="rare", 0.792892156862745, 1)))</f>
@@ -6685,7 +6685,7 @@
         <v>0.06</v>
       </c>
       <c r="E116" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F116" s="3">
         <f>IF(B116:B324="common", 4, IF(B116:B324="uncommon", 3, IF(B116:B324="rare", 0.792892156862745, 1)))</f>
@@ -6735,10 +6735,10 @@
         <v>21</v>
       </c>
       <c r="D117" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="E117" s="3" t="n">
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
       <c r="F117" s="3">
         <f>IF(B117:B325="common", 4, IF(B117:B325="uncommon", 3, IF(B117:B325="rare", 0.792892156862745, 1)))</f>
@@ -6788,7 +6788,7 @@
         <v>46</v>
       </c>
       <c r="D118" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E118" s="3" t="n">
         <v>0.17</v>
@@ -6841,10 +6841,10 @@
         <v>46</v>
       </c>
       <c r="D119" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E119" s="3" t="n">
-        <v>2.56</v>
+        <v>2.39</v>
       </c>
       <c r="F119" s="3">
         <f>IF(B119:B327="common", 4, IF(B119:B327="uncommon", 3, IF(B119:B327="rare", 0.792892156862745, 1)))</f>
@@ -6894,7 +6894,7 @@
         <v>90</v>
       </c>
       <c r="D120" s="3" t="n">
-        <v>6.36</v>
+        <v>6.59</v>
       </c>
       <c r="E120" s="3" t="inlineStr"/>
       <c r="F120" s="3">
@@ -6945,7 +6945,7 @@
         <v>248</v>
       </c>
       <c r="D121" s="3" t="n">
-        <v>17.12</v>
+        <v>17.23</v>
       </c>
       <c r="E121" s="3" t="inlineStr"/>
       <c r="F121" s="3">
@@ -6996,7 +6996,7 @@
         <v>154</v>
       </c>
       <c r="D122" s="3" t="n">
-        <v>12</v>
+        <v>11.79</v>
       </c>
       <c r="E122" s="3" t="inlineStr"/>
       <c r="F122" s="3">
@@ -7047,7 +7047,7 @@
         <v>90</v>
       </c>
       <c r="D123" s="3" t="n">
-        <v>9.630000000000001</v>
+        <v>9.19</v>
       </c>
       <c r="E123" s="3" t="inlineStr"/>
       <c r="F123" s="3">
@@ -7098,10 +7098,10 @@
         <v>21</v>
       </c>
       <c r="D124" s="3" t="n">
-        <v>0.47</v>
+        <v>0.7</v>
       </c>
       <c r="E124" s="3" t="n">
-        <v>1.46</v>
+        <v>1.24</v>
       </c>
       <c r="F124" s="3">
         <f>IF(B124:B332="common", 4, IF(B124:B332="uncommon", 3, IF(B124:B332="rare", 0.792892156862745, 1)))</f>
@@ -7151,10 +7151,10 @@
         <v>21</v>
       </c>
       <c r="D125" s="3" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="E125" s="3" t="n">
-        <v>0.64</v>
+        <v>0.59</v>
       </c>
       <c r="F125" s="3">
         <f>IF(B125:B333="common", 4, IF(B125:B333="uncommon", 3, IF(B125:B333="rare", 0.792892156862745, 1)))</f>
@@ -7257,7 +7257,7 @@
         <v>188</v>
       </c>
       <c r="D127" s="3" t="n">
-        <v>5.29</v>
+        <v>5.61</v>
       </c>
       <c r="E127" s="3" t="inlineStr"/>
       <c r="F127" s="3">
@@ -7361,7 +7361,7 @@
         <v>21</v>
       </c>
       <c r="D129" s="3" t="n">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="E129" s="3" t="n">
         <v>0.7</v>
@@ -7414,7 +7414,7 @@
         <v>188</v>
       </c>
       <c r="D130" s="3" t="n">
-        <v>9.15</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="E130" s="3" t="inlineStr"/>
       <c r="F130" s="3">
@@ -7465,7 +7465,7 @@
         <v>33</v>
       </c>
       <c r="D131" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E131" s="3" t="n">
         <v>0.19</v>
@@ -7521,7 +7521,7 @@
         <v>0.13</v>
       </c>
       <c r="E132" s="3" t="n">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="F132" s="3">
         <f>IF(B132:B340="common", 4, IF(B132:B340="uncommon", 3, IF(B132:B340="rare", 0.792892156862745, 1)))</f>
@@ -7571,10 +7571,10 @@
         <v>46</v>
       </c>
       <c r="D133" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E133" s="3" t="n">
-        <v>1.19</v>
+        <v>1.22</v>
       </c>
       <c r="F133" s="3">
         <f>IF(B133:B341="common", 4, IF(B133:B341="uncommon", 3, IF(B133:B341="rare", 0.792892156862745, 1)))</f>
@@ -7677,7 +7677,7 @@
         <v>33</v>
       </c>
       <c r="D135" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E135" s="3" t="n">
         <v>0.16</v>
@@ -7730,7 +7730,7 @@
         <v>90</v>
       </c>
       <c r="D136" s="3" t="n">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
       <c r="E136" s="3" t="inlineStr"/>
       <c r="F136" s="3">
@@ -7781,7 +7781,7 @@
         <v>248</v>
       </c>
       <c r="D137" s="3" t="n">
-        <v>7.36</v>
+        <v>7.28</v>
       </c>
       <c r="E137" s="3" t="inlineStr"/>
       <c r="F137" s="3">
@@ -7835,7 +7835,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E138" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F138" s="3">
         <f>IF(B138:B346="common", 4, IF(B138:B346="uncommon", 3, IF(B138:B346="rare", 0.792892156862745, 1)))</f>
@@ -7885,10 +7885,10 @@
         <v>33</v>
       </c>
       <c r="D139" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E139" s="3" t="n">
-        <v>1.69</v>
+        <v>1.6</v>
       </c>
       <c r="F139" s="3">
         <f>IF(B139:B347="common", 4, IF(B139:B347="uncommon", 3, IF(B139:B347="rare", 0.792892156862745, 1)))</f>
@@ -7938,7 +7938,7 @@
         <v>188</v>
       </c>
       <c r="D140" s="3" t="n">
-        <v>5.75</v>
+        <v>5.69</v>
       </c>
       <c r="E140" s="3" t="inlineStr"/>
       <c r="F140" s="3">
@@ -7989,10 +7989,10 @@
         <v>21</v>
       </c>
       <c r="D141" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="E141" s="3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="F141" s="3">
         <f>IF(B141:B349="common", 4, IF(B141:B349="uncommon", 3, IF(B141:B349="rare", 0.792892156862745, 1)))</f>
@@ -8042,10 +8042,10 @@
         <v>33</v>
       </c>
       <c r="D142" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E142" s="3" t="n">
-        <v>1.41</v>
+        <v>1.42</v>
       </c>
       <c r="F142" s="3">
         <f>IF(B142:B350="common", 4, IF(B142:B350="uncommon", 3, IF(B142:B350="rare", 0.792892156862745, 1)))</f>
@@ -8095,7 +8095,7 @@
         <v>46</v>
       </c>
       <c r="D143" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E143" s="3" t="n">
         <v>0.15</v>
@@ -8148,7 +8148,7 @@
         <v>33</v>
       </c>
       <c r="D144" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E144" s="3" t="n">
         <v>0.16</v>
@@ -8204,7 +8204,7 @@
         <v>0.05</v>
       </c>
       <c r="E145" s="3" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="F145" s="3">
         <f>IF(B145:B353="common", 4, IF(B145:B353="uncommon", 3, IF(B145:B353="rare", 0.792892156862745, 1)))</f>
@@ -8257,7 +8257,7 @@
         <v>0.08</v>
       </c>
       <c r="E146" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F146" s="3">
         <f>IF(B146:B354="common", 4, IF(B146:B354="uncommon", 3, IF(B146:B354="rare", 0.792892156862745, 1)))</f>
@@ -8307,10 +8307,10 @@
         <v>46</v>
       </c>
       <c r="D147" s="3" t="n">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>2.4</v>
+        <v>2.42</v>
       </c>
       <c r="F147" s="3">
         <f>IF(B147:B355="common", 4, IF(B147:B355="uncommon", 3, IF(B147:B355="rare", 0.792892156862745, 1)))</f>
@@ -8363,7 +8363,7 @@
         <v>0.1</v>
       </c>
       <c r="E148" s="3" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
       <c r="F148" s="3">
         <f>IF(B148:B356="common", 4, IF(B148:B356="uncommon", 3, IF(B148:B356="rare", 0.792892156862745, 1)))</f>
@@ -8466,7 +8466,7 @@
         <v>188</v>
       </c>
       <c r="D150" s="3" t="n">
-        <v>24.78</v>
+        <v>25.64</v>
       </c>
       <c r="E150" s="3" t="inlineStr"/>
       <c r="F150" s="3">
@@ -8520,7 +8520,7 @@
         <v>0.06</v>
       </c>
       <c r="E151" s="3" t="n">
-        <v>1.42</v>
+        <v>1.41</v>
       </c>
       <c r="F151" s="3">
         <f>IF(B151:B359="common", 4, IF(B151:B359="uncommon", 3, IF(B151:B359="rare", 0.792892156862745, 1)))</f>
@@ -8570,7 +8570,7 @@
         <v>46</v>
       </c>
       <c r="D152" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E152" s="3" t="n">
         <v>0.13</v>
@@ -8626,7 +8626,7 @@
         <v>0.12</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>1.79</v>
+        <v>1.61</v>
       </c>
       <c r="F153" s="3">
         <f>IF(B153:B361="common", 4, IF(B153:B361="uncommon", 3, IF(B153:B361="rare", 0.792892156862745, 1)))</f>
@@ -8676,7 +8676,7 @@
         <v>188</v>
       </c>
       <c r="D154" s="3" t="n">
-        <v>16.93</v>
+        <v>17.12</v>
       </c>
       <c r="E154" s="3" t="inlineStr"/>
       <c r="F154" s="3">
@@ -8727,10 +8727,10 @@
         <v>33</v>
       </c>
       <c r="D155" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E155" s="3" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F155" s="3">
         <f>IF(B155:B363="common", 4, IF(B155:B363="uncommon", 3, IF(B155:B363="rare", 0.792892156862745, 1)))</f>
@@ -8780,7 +8780,7 @@
         <v>46</v>
       </c>
       <c r="D156" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E156" s="3" t="n">
         <v>0.12</v>
@@ -8942,7 +8942,7 @@
         <v>0.13</v>
       </c>
       <c r="E159" s="3" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="F159" s="3">
         <f>IF(B159:B367="common", 4, IF(B159:B367="uncommon", 3, IF(B159:B367="rare", 0.792892156862745, 1)))</f>
@@ -8992,10 +8992,10 @@
         <v>46</v>
       </c>
       <c r="D160" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E160" s="3" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="F160" s="3">
         <f>IF(B160:B368="common", 4, IF(B160:B368="uncommon", 3, IF(B160:B368="rare", 0.792892156862745, 1)))</f>
@@ -9045,7 +9045,7 @@
         <v>188</v>
       </c>
       <c r="D161" s="3" t="n">
-        <v>18.6</v>
+        <v>19.17</v>
       </c>
       <c r="E161" s="3" t="inlineStr"/>
       <c r="F161" s="3">
@@ -9099,7 +9099,7 @@
         <v>0.13</v>
       </c>
       <c r="E162" s="3" t="n">
-        <v>1.21</v>
+        <v>1.23</v>
       </c>
       <c r="F162" s="3">
         <f>IF(B162:B370="common", 4, IF(B162:B370="uncommon", 3, IF(B162:B370="rare", 0.792892156862745, 1)))</f>
@@ -9149,7 +9149,7 @@
         <v>33</v>
       </c>
       <c r="D163" s="3" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E163" s="3" t="n">
         <v>0.13</v>
@@ -9205,7 +9205,7 @@
         <v>0.06</v>
       </c>
       <c r="E164" s="3" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="F164" s="3">
         <f>IF(B164:B372="common", 4, IF(B164:B372="uncommon", 3, IF(B164:B372="rare", 0.792892156862745, 1)))</f>
@@ -9255,7 +9255,7 @@
         <v>46</v>
       </c>
       <c r="D165" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E165" s="3" t="n">
         <v>0.16</v>
@@ -9361,7 +9361,7 @@
         <v>46</v>
       </c>
       <c r="D167" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E167" s="3" t="n">
         <v>0.12</v>
@@ -9414,7 +9414,7 @@
         <v>33</v>
       </c>
       <c r="D168" s="3" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="E168" s="3" t="n">
         <v>0.89</v>
@@ -9467,7 +9467,7 @@
         <v>46</v>
       </c>
       <c r="D169" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E169" s="3" t="n">
         <v>0.17</v>
@@ -9520,7 +9520,7 @@
         <v>33</v>
       </c>
       <c r="D170" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E170" s="3" t="n">
         <v>0.15</v>
@@ -9573,10 +9573,10 @@
         <v>33</v>
       </c>
       <c r="D171" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="E171" s="3" t="n">
-        <v>2.37</v>
+        <v>2.3</v>
       </c>
       <c r="F171" s="3">
         <f>IF(B171:B379="common", 4, IF(B171:B379="uncommon", 3, IF(B171:B379="rare", 0.792892156862745, 1)))</f>
@@ -9626,10 +9626,10 @@
         <v>33</v>
       </c>
       <c r="D172" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E172" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F172" s="3">
         <f>IF(B172:B380="common", 4, IF(B172:B380="uncommon", 3, IF(B172:B380="rare", 0.792892156862745, 1)))</f>
@@ -9679,10 +9679,10 @@
         <v>33</v>
       </c>
       <c r="D173" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E173" s="3" t="n">
-        <v>0.97</v>
+        <v>0.87</v>
       </c>
       <c r="F173" s="3">
         <f>IF(B173:B381="common", 4, IF(B173:B381="uncommon", 3, IF(B173:B381="rare", 0.792892156862745, 1)))</f>
@@ -9788,7 +9788,7 @@
         <v>0.06</v>
       </c>
       <c r="E175" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F175" s="3">
         <f>IF(B175:B383="common", 4, IF(B175:B383="uncommon", 3, IF(B175:B383="rare", 0.792892156862745, 1)))</f>
@@ -9838,7 +9838,7 @@
         <v>33</v>
       </c>
       <c r="D176" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E176" s="3" t="n">
         <v>0.15</v>
@@ -9891,10 +9891,10 @@
         <v>46</v>
       </c>
       <c r="D177" s="3" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E177" s="3" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="F177" s="3">
         <f>IF(B177:B385="common", 4, IF(B177:B385="uncommon", 3, IF(B177:B385="rare", 0.792892156862745, 1)))</f>
@@ -9947,7 +9947,7 @@
         <v>0.12</v>
       </c>
       <c r="E178" s="3" t="n">
-        <v>1.19</v>
+        <v>1.08</v>
       </c>
       <c r="F178" s="3">
         <f>IF(B178:B386="common", 4, IF(B178:B386="uncommon", 3, IF(B178:B386="rare", 0.792892156862745, 1)))</f>
@@ -10000,7 +10000,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E179" s="3" t="n">
-        <v>1.06</v>
+        <v>1.09</v>
       </c>
       <c r="F179" s="3">
         <f>IF(B179:B387="common", 4, IF(B179:B387="uncommon", 3, IF(B179:B387="rare", 0.792892156862745, 1)))</f>
@@ -10050,7 +10050,7 @@
         <v>46</v>
       </c>
       <c r="D180" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E180" s="3" t="n">
         <v>0.18</v>
@@ -10103,7 +10103,7 @@
         <v>188</v>
       </c>
       <c r="D181" s="3" t="n">
-        <v>38.56</v>
+        <v>38.24</v>
       </c>
       <c r="E181" s="3" t="inlineStr"/>
       <c r="F181" s="3">
@@ -10154,10 +10154,10 @@
         <v>21</v>
       </c>
       <c r="D182" s="3" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="E182" s="3" t="n">
-        <v>0.57</v>
+        <v>0.63</v>
       </c>
       <c r="F182" s="3">
         <f>IF(B182:B390="common", 4, IF(B182:B390="uncommon", 3, IF(B182:B390="rare", 0.792892156862745, 1)))</f>
@@ -10260,7 +10260,7 @@
         <v>154</v>
       </c>
       <c r="D184" s="3" t="n">
-        <v>2.16</v>
+        <v>2.12</v>
       </c>
       <c r="E184" s="3" t="inlineStr"/>
       <c r="F184" s="3">
@@ -10311,10 +10311,10 @@
         <v>46</v>
       </c>
       <c r="D185" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E185" s="3" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="F185" s="3">
         <f>IF(B185:B393="common", 4, IF(B185:B393="uncommon", 3, IF(B185:B393="rare", 0.792892156862745, 1)))</f>
@@ -10364,7 +10364,7 @@
         <v>188</v>
       </c>
       <c r="D186" s="3" t="n">
-        <v>6.47</v>
+        <v>6.86</v>
       </c>
       <c r="E186" s="3" t="inlineStr"/>
       <c r="F186" s="3">
@@ -10418,7 +10418,7 @@
         <v>0.1</v>
       </c>
       <c r="E187" s="3" t="n">
-        <v>0.85</v>
+        <v>0.79</v>
       </c>
       <c r="F187" s="3">
         <f>IF(B187:B395="common", 4, IF(B187:B395="uncommon", 3, IF(B187:B395="rare", 0.792892156862745, 1)))</f>
@@ -10577,7 +10577,7 @@
         <v>0.22</v>
       </c>
       <c r="E190" s="3" t="n">
-        <v>1.31</v>
+        <v>1.45</v>
       </c>
       <c r="F190" s="3">
         <f>IF(B190:B398="common", 4, IF(B190:B398="uncommon", 3, IF(B190:B398="rare", 0.792892156862745, 1)))</f>
@@ -10630,7 +10630,7 @@
         <v>0.08</v>
       </c>
       <c r="E191" s="3" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="F191" s="3">
         <f>IF(B191:B399="common", 4, IF(B191:B399="uncommon", 3, IF(B191:B399="rare", 0.792892156862745, 1)))</f>
@@ -10733,7 +10733,7 @@
         <v>90</v>
       </c>
       <c r="D193" s="3" t="n">
-        <v>0.73</v>
+        <v>0.6</v>
       </c>
       <c r="E193" s="3" t="inlineStr"/>
       <c r="F193" s="3">
@@ -10784,7 +10784,7 @@
         <v>248</v>
       </c>
       <c r="D194" s="3" t="n">
-        <v>9.5</v>
+        <v>9.59</v>
       </c>
       <c r="E194" s="3" t="inlineStr"/>
       <c r="F194" s="3">
@@ -10835,7 +10835,7 @@
         <v>225</v>
       </c>
       <c r="D195" s="3" t="n">
-        <v>57.55</v>
+        <v>58.02</v>
       </c>
       <c r="E195" s="3" t="inlineStr"/>
       <c r="F195" s="3">
@@ -10939,10 +10939,10 @@
         <v>21</v>
       </c>
       <c r="D197" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="E197" s="3" t="n">
-        <v>0.77</v>
+        <v>0.68</v>
       </c>
       <c r="F197" s="3">
         <f>IF(B197:B405="common", 4, IF(B197:B405="uncommon", 3, IF(B197:B405="rare", 0.792892156862745, 1)))</f>
@@ -10992,7 +10992,7 @@
         <v>46</v>
       </c>
       <c r="D198" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E198" s="3" t="n">
         <v>0.13</v>
@@ -11098,10 +11098,10 @@
         <v>33</v>
       </c>
       <c r="D200" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E200" s="3" t="n">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="F200" s="3">
         <f>IF(B200:B408="common", 4, IF(B200:B408="uncommon", 3, IF(B200:B408="rare", 0.792892156862745, 1)))</f>
@@ -11151,7 +11151,7 @@
         <v>188</v>
       </c>
       <c r="D201" s="3" t="n">
-        <v>23.06</v>
+        <v>23.62</v>
       </c>
       <c r="E201" s="3" t="inlineStr"/>
       <c r="F201" s="3">
@@ -11205,7 +11205,7 @@
         <v>0.05</v>
       </c>
       <c r="E202" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F202" s="3">
         <f>IF(B202:B410="common", 4, IF(B202:B410="uncommon", 3, IF(B202:B410="rare", 0.792892156862745, 1)))</f>
@@ -11255,10 +11255,10 @@
         <v>46</v>
       </c>
       <c r="D203" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E203" s="3" t="n">
-        <v>1.47</v>
+        <v>1.4</v>
       </c>
       <c r="F203" s="3">
         <f>IF(B203:B411="common", 4, IF(B203:B411="uncommon", 3, IF(B203:B411="rare", 0.792892156862745, 1)))</f>
@@ -11308,10 +11308,10 @@
         <v>21</v>
       </c>
       <c r="D204" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="E204" s="3" t="n">
-        <v>0.74</v>
+        <v>0.72</v>
       </c>
       <c r="F204" s="3">
         <f>IF(B204:B412="common", 4, IF(B204:B412="uncommon", 3, IF(B204:B412="rare", 0.792892156862745, 1)))</f>
@@ -11361,7 +11361,7 @@
         <v>90</v>
       </c>
       <c r="D205" s="3" t="n">
-        <v>0.74</v>
+        <v>0.62</v>
       </c>
       <c r="E205" s="3" t="inlineStr"/>
       <c r="F205" s="3">
@@ -11412,7 +11412,7 @@
         <v>248</v>
       </c>
       <c r="D206" s="3" t="n">
-        <v>6.46</v>
+        <v>6.01</v>
       </c>
       <c r="E206" s="3" t="inlineStr"/>
       <c r="F206" s="3">
@@ -11463,7 +11463,7 @@
         <v>90</v>
       </c>
       <c r="D207" s="3" t="n">
-        <v>0.8</v>
+        <v>0.68</v>
       </c>
       <c r="E207" s="3" t="inlineStr"/>
       <c r="F207" s="3">
@@ -11514,7 +11514,7 @@
         <v>248</v>
       </c>
       <c r="D208" s="3" t="n">
-        <v>7.29</v>
+        <v>7.19</v>
       </c>
       <c r="E208" s="3" t="inlineStr"/>
       <c r="F208" s="3">
@@ -11565,7 +11565,7 @@
         <v>225</v>
       </c>
       <c r="D209" s="3" t="n">
-        <v>47.08</v>
+        <v>47.43</v>
       </c>
       <c r="E209" s="3" t="inlineStr"/>
       <c r="F209" s="3">
@@ -11616,10 +11616,10 @@
         <v>46</v>
       </c>
       <c r="D210" s="3" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="E210" s="3" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="F210" s="3">
         <f>IF(B210:B418="common", 4, IF(B210:B418="uncommon", 3, IF(B210:B418="rare", 0.792892156862745, 1)))</f>
@@ -18308,7 +18308,7 @@
         </is>
       </c>
       <c r="B2" s="13" t="n">
-        <v>0.4</v>
+        <v>0.3956521739130435</v>
       </c>
     </row>
     <row r="3">
@@ -18318,7 +18318,7 @@
         </is>
       </c>
       <c r="B3" s="13" t="n">
-        <v>0.4518181818181817</v>
+        <v>0.4836363636363635</v>
       </c>
     </row>
     <row r="4">
@@ -18328,7 +18328,7 @@
         </is>
       </c>
       <c r="B4" s="13" t="n">
-        <v>0.192937091503268</v>
+        <v>0.1940697945845005</v>
       </c>
     </row>
     <row r="5">
@@ -18338,7 +18338,7 @@
         </is>
       </c>
       <c r="B5" s="13" t="n">
-        <v>5.184226906095112</v>
+        <v>5.106821201141853</v>
       </c>
     </row>
     <row r="6">
@@ -18378,7 +18378,7 @@
         </is>
       </c>
       <c r="B9" s="13" t="n">
-        <v>1.717021276595745</v>
+        <v>1.732659574468085</v>
       </c>
     </row>
     <row r="10">
@@ -18388,7 +18388,7 @@
         </is>
       </c>
       <c r="B10" s="13" t="n">
-        <v>1.917377777777778</v>
+        <v>1.924355555555556</v>
       </c>
     </row>
     <row r="11">
@@ -18398,7 +18398,7 @@
         </is>
       </c>
       <c r="B11" s="13" t="n">
-        <v>0.3141111111111111</v>
+        <v>0.3109999999999999</v>
       </c>
     </row>
     <row r="12">
@@ -18408,7 +18408,7 @@
         </is>
       </c>
       <c r="B12" s="13" t="n">
-        <v>0.1208441558441558</v>
+        <v>0.1167532467532467</v>
       </c>
     </row>
     <row r="13">
@@ -18418,7 +18418,7 @@
         </is>
       </c>
       <c r="B13" s="13" t="n">
-        <v>0.5269354838709677</v>
+        <v>0.517983870967742</v>
       </c>
     </row>
     <row r="14">
@@ -18448,7 +18448,7 @@
         </is>
       </c>
       <c r="B16" s="13" t="n">
-        <v>4.596289805199757</v>
+        <v>4.602752247744629</v>
       </c>
     </row>
     <row r="17">
@@ -18458,7 +18458,7 @@
         </is>
       </c>
       <c r="B17" s="13" t="n">
-        <v>10.82527198461632</v>
+        <v>10.78293178102039</v>
       </c>
     </row>
     <row r="18">
@@ -18468,7 +18468,7 @@
         </is>
       </c>
       <c r="B18" s="13" t="n">
-        <v>0.9352719846163176</v>
+        <v>0.7929317810203909</v>
       </c>
     </row>
     <row r="19">
@@ -18478,7 +18478,7 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>1.094567440304987</v>
+        <v>1.079372550652692</v>
       </c>
     </row>
     <row r="20">
@@ -18488,7 +18488,7 @@
         </is>
       </c>
       <c r="B20" s="15" t="n">
-        <v>0.09456744030498655</v>
+        <v>0.07937255065269189</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
currently working code, needs refractoring.
</commit_message>
<xml_diff>
--- a/excelDocs/scarletAndViolet151/pokemon_data.xlsx
+++ b/excelDocs/scarletAndViolet151/pokemon_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EVRCalculator\excelDocs\scarletAndViolet151\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6A47B9-705C-4B40-AAD0-B34C7560F1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4908A4B-A8B5-4EC8-A869-F562AE649E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="1605" windowWidth="25260" windowHeight="11385" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:AY1263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>